<commit_message>
quality analysis of camera configs
</commit_message>
<xml_diff>
--- a/cis_541/Project1/F_CDUX/Camera Positions Results.xlsx
+++ b/cis_541/Project1/F_CDUX/Camera Positions Results.xlsx
@@ -320,20 +320,20 @@
   <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J46" activeCellId="0" sqref="J46"/>
+      <selection pane="topLeft" activeCell="H32" activeCellId="0" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="33.6122448979592"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="49.8112244897959"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="35.3673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="49.2704081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="34.9642857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -354,6 +354,7 @@
       <c r="G1" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="H1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3"/>
@@ -363,6 +364,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="3"/>
       <c r="G2" s="5"/>
+      <c r="H2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0"/>
@@ -374,6 +376,7 @@
       <c r="G3" s="6" t="s">
         <v>5</v>
       </c>
+      <c r="H3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -1644,6 +1647,7 @@
       <c r="E67" s="0"/>
       <c r="F67" s="0"/>
       <c r="G67" s="0"/>
+      <c r="H67" s="0"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="8" t="n">

</xml_diff>

<commit_message>
getting started with 2B
</commit_message>
<xml_diff>
--- a/cis_541/Project1/F_CDUX/Camera Positions Results.xlsx
+++ b/cis_541/Project1/F_CDUX/Camera Positions Results.xlsx
@@ -187,7 +187,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -218,6 +218,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -320,7 +324,7 @@
   <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H32" activeCellId="0" sqref="H32"/>
+      <selection pane="topLeft" activeCell="H27" activeCellId="0" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -778,7 +782,7 @@
         <v>2749335</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>21</v>
       </c>
@@ -796,7 +800,7 @@
       <c r="G24" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H24" s="1" t="n">
+      <c r="H24" s="8" t="n">
         <v>4116191</v>
       </c>
     </row>
@@ -1650,36 +1654,36 @@
       <c r="H67" s="0"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="8" t="n">
+      <c r="B68" s="9" t="n">
         <f aca="false">MAX(B4:B66)</f>
         <v>6650005</v>
       </c>
-      <c r="D68" s="9" t="n">
+      <c r="D68" s="10" t="n">
         <f aca="false">MAX(D4:D66)</f>
         <v>238783</v>
       </c>
-      <c r="F68" s="10" t="n">
+      <c r="F68" s="11" t="n">
         <f aca="false">MAX(F4:F66)</f>
         <v>2125239</v>
       </c>
-      <c r="G68" s="11" t="n">
+      <c r="G68" s="12" t="n">
         <f aca="false">MAX(B68, D68, F68)</f>
         <v>6650005</v>
       </c>
-      <c r="H68" s="12" t="n">
+      <c r="H68" s="13" t="n">
         <f aca="false">MAX(H4:H66)</f>
         <v>4116191</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="8"/>
-      <c r="D69" s="9"/>
-      <c r="F69" s="10"/>
-      <c r="G69" s="11"/>
-      <c r="H69" s="12"/>
+      <c r="B69" s="9"/>
+      <c r="D69" s="10"/>
+      <c r="F69" s="11"/>
+      <c r="G69" s="12"/>
+      <c r="H69" s="13"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G70" s="11" t="n">
+      <c r="G70" s="12" t="n">
         <f aca="false">F68</f>
         <v>2125239</v>
       </c>

</xml_diff>